<commit_message>
Update excel for thunderbird
</commit_message>
<xml_diff>
--- a/Analysis/ThunderbirdStats.xlsx
+++ b/Analysis/ThunderbirdStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\MGL870-TP2-Remise\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A73F6A6-3F20-4B2D-B974-4E57D2CDC1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB896A6-3751-4217-B9DF-A8A89D750234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Stats" sheetId="1" r:id="rId1"/>
@@ -26,32 +26,27 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'Data Stats'!$B$7:$B$11</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'Data Stats'!$C$7:$C$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'RF+RL 10M'!$C$9:$C$33</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'RF+RL 10M'!$D$9:$D$33</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'RF+RL 10M'!$E$8</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'RF+RL 10M'!$E$9:$E$33</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'RF-Box &amp; Whisker 10M'!$D$8:$D$27</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'RF-Box &amp; Whisker 10M'!$E$7</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'RF-Box &amp; Whisker 10M'!$E$8:$E$27</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'LR-Box &amp; Whisker 10M'!$D$9:$E$28</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'LR-Box &amp; Whisker 10M'!$F$8</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'LR-Box &amp; Whisker 10M'!$F$9:$F$28</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'RF-Box &amp; Whisker 10M'!$E$7</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'RF-Box &amp; Whisker 10M'!$E$8:$E$27</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'LR-Box &amp; Whisker 10M'!$D$9:$E$28</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'LR-Box &amp; Whisker 10M'!$F$8</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'LR-Box &amp; Whisker 10M'!$F$9:$F$28</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'RF-Box &amp; Whisker 20M'!$D$9:$D$28</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'RF-Box &amp; Whisker 20M'!$E$8</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'RF-Box &amp; Whisker 20M'!$E$9:$E$28</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'LR-Box &amp; Whisker 20M'!$D$9:$D$28</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'LR-Box &amp; Whisker 20M'!$E$8</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'Data Stats'!$A$7:$A$11</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'RF-Box &amp; Whisker 20M'!$D$9:$D$28</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'RF-Box &amp; Whisker 20M'!$E$8</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'RF-Box &amp; Whisker 20M'!$E$9:$E$28</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'LR-Box &amp; Whisker 20M'!$D$9:$D$28</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'LR-Box &amp; Whisker 20M'!$E$8</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'LR-Box &amp; Whisker 20M'!$E$9:$E$28</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Others!$J$8:$J$12</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Others!$K$8:$K$12</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'LR-Box &amp; Whisker 20M'!$E$9:$E$28</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Others!$J$8:$J$12</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Others!$K$8:$K$12</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Data Stats'!$C$7:$C$11</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'RF+RL 10M'!$C$8</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'RF+RL 10M'!$C$9:$C$33</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'RF+RL 10M'!$D$9:$D$33</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'RF+RL 10M'!$E$8</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">'RF+RL 10M'!$E$9:$E$33</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'RF+RL 10M'!$C$8</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'RF-Box &amp; Whisker 10M'!$D$8:$D$27</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -63,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="61">
   <si>
     <t>CPU</t>
   </si>
@@ -243,6 +238,9 @@
   </si>
   <si>
     <t>3600 1800 60</t>
+  </si>
+  <si>
+    <t>Importance [0-1]</t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1182,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1245,7 +1243,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6899912A-E712-44A0-B8B2-BB8F0EF76B29}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.15</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Score</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1335,10 +1333,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1378,7 +1376,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{3E6BAE52-1607-448C-85FD-404D4B066EAD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.13</cx:f>
               <cx:v>Score</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1463,10 +1461,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.20</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.22</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1496,7 +1494,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{202117BA-FFDA-4949-A405-F197D342C9FE}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.21</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>Score</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1529,10 +1527,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.18</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.25</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1562,7 +1560,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{CEA85BE7-71CD-4691-82E3-D870ADC49C46}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.24</cx:f>
+              <cx:f>_xlchart.v1.19</cx:f>
               <cx:v>Score</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1595,10 +1593,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.27</cx:f>
+        <cx:f>_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -7883,7 +7881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1483A604-DE0A-4BDE-9BBE-72617D0A450A}">
   <dimension ref="A7:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -8846,8 +8844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCE905A-2CF5-4379-993D-5BFAA27A5D4D}">
   <dimension ref="C6:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8887,7 +8885,7 @@
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>41</v>

</xml_diff>